<commit_message>
Arreglo de archivos: Acta y Backlog
</commit_message>
<xml_diff>
--- a/documetacionSoftware/1. Inicio/Backlog del producto.xlsx
+++ b/documetacionSoftware/1. Inicio/Backlog del producto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjmasache/Documents/quintoCiclo/ingenieriaSoftware/proyecto/Plantillas de Gestión de Proyecto/01. INICIO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sant Garcia\Documents\5to Ciclo\proyectoCromos\documetacionSoftware\1. Inicio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E23422B-5EF5-BE41-B0CC-FE87A5BBF814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9FF6C8-578A-4060-BF5B-1D47217D141F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog del Producto" sheetId="8" r:id="rId1"/>
@@ -31,13 +31,13 @@
     <definedName name="PBCurrentBottom">OFFSET(#REF!,1,0,#REF!,1)</definedName>
     <definedName name="PBTrend">OFFSET(#REF!,1,0,#REF!,1)</definedName>
     <definedName name="PlannedSpeed">OFFSET(#REF!,1,0,#REF!,1)</definedName>
-    <definedName name="ProductBacklog">'Backlog del Producto'!$B$5:$P$190</definedName>
+    <definedName name="ProductBacklog">'Backlog del Producto'!$B$5:$P$187</definedName>
     <definedName name="RealizedSpeed">OFFSET(#REF!,1,0,#REF!,1)</definedName>
-    <definedName name="Sprint">'Backlog del Producto'!$N$7:$N$190</definedName>
+    <definedName name="Sprint">'Backlog del Producto'!$N$21:$N$187</definedName>
     <definedName name="SprintCount">#REF!</definedName>
     <definedName name="SprintsInTrend">#REF!</definedName>
     <definedName name="SprintTasks">#REF!</definedName>
-    <definedName name="Status">'Backlog del Producto'!$O$7:$O$190</definedName>
+    <definedName name="Status">'Backlog del Producto'!$O$21:$O$187</definedName>
     <definedName name="StoryName">'Backlog del Producto'!#REF!</definedName>
     <definedName name="TaskRows">#REF!</definedName>
     <definedName name="TaskStatus">#REF!</definedName>
@@ -55,7 +55,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -188,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
   <si>
     <t>Backlog del Producto</t>
   </si>
@@ -271,16 +270,10 @@
     <t>Gestor del sistema</t>
   </si>
   <si>
-    <t>Poder registrar los usuarios en la aplicación</t>
-  </si>
-  <si>
     <t>Asignar las preguntas y los cromos en la cantidad respectiva</t>
   </si>
   <si>
     <t>HU01</t>
-  </si>
-  <si>
-    <t>Deseo poder registrar de manera correcta cada uno de los usuarios con los datos sus datos respectivos</t>
   </si>
   <si>
     <t>Controlar correctamente su acceso al sistema</t>
@@ -293,9 +286,6 @@
     <t>HU02</t>
   </si>
   <si>
-    <t>Deseo poder realizar la asignación automatizada y aleatoria de las preguntas para el usuario</t>
-  </si>
-  <si>
     <t xml:space="preserve">Evitar el descontrol en la repartición y repetición de preguntas </t>
   </si>
   <si>
@@ -306,9 +296,6 @@
     <t>HU03</t>
   </si>
   <si>
-    <t>Deseo poder generar la cantidad acorde y limitada de cromos en funció de las respuestas correctas del usuario</t>
-  </si>
-  <si>
     <t>Impedir el exceso de cromos que se pueden conseguir diariamente</t>
   </si>
   <si>
@@ -319,9 +306,6 @@
     <t>HU04</t>
   </si>
   <si>
-    <t>Deseo poder visualizar el progreso de cada usuario tanto en sus temáticas como en su álbum digital</t>
-  </si>
-  <si>
     <t>Para tener un seguimiento de aprendizaje de los usuarios</t>
   </si>
   <si>
@@ -368,9 +352,6 @@
     <t>Que puedan ser consumidas/tomadas y/o actualizadas</t>
   </si>
   <si>
-    <t>Poder realizar la carga de información dentro de la base de datos de la aplicación</t>
-  </si>
-  <si>
     <t>Cargar las preguntas en base a las temáticas respectivas</t>
   </si>
   <si>
@@ -391,41 +372,87 @@
 2. La cantidad de cromos no debe exceder el valor de 180</t>
   </si>
   <si>
-    <t>Cliente/ Dueño del producto</t>
-  </si>
-  <si>
-    <t>Poder visualizar el funcionamiento correcto del sistema (a nivel de usuario)</t>
-  </si>
-  <si>
-    <t>Gestionar el envío de la información correspondiente</t>
-  </si>
-  <si>
     <t>Dueño del producto</t>
   </si>
   <si>
-    <t>Gestionar y enviar las preguntas de todas las temáticas a abordar</t>
-  </si>
-  <si>
-    <t>Gestionar y enviar los cromos de todas las temáticas a abordar</t>
-  </si>
-  <si>
-    <t>Su respectiva carga en la aplicación</t>
-  </si>
-  <si>
-    <t>Deben poseer un formato que acepte la aplicación para su respectiva carga</t>
-  </si>
-  <si>
-    <t>La información debe ser clara y poseer un formato que acepte la aplicación para su respectiva carga</t>
-  </si>
-  <si>
     <t>Por hacer</t>
+  </si>
+  <si>
+    <t>EPIC04</t>
+  </si>
+  <si>
+    <t>Que cada usuario mantenga un progreso integro conforme a progreso</t>
+  </si>
+  <si>
+    <t>Integridad del progreso del usuario conforme a sus cromos obtenidos</t>
+  </si>
+  <si>
+    <t>1. Se debe guardar la informacion de cada cromo obtenido
+2. Se debe guardar la cantidad de cromos obtenidos</t>
+  </si>
+  <si>
+    <t>EPIC01-HU01</t>
+  </si>
+  <si>
+    <t>Registrar de manera correcta cada uno de los usuarios con los datos sus datos respectivos</t>
+  </si>
+  <si>
+    <t>Registrar los usuarios en la aplicación</t>
+  </si>
+  <si>
+    <t>Realizar la carga de información dentro de la base de datos de la aplicación</t>
+  </si>
+  <si>
+    <t>Crear y mantener la estructura de un album digital por cada usuario del sistema</t>
+  </si>
+  <si>
+    <t>Visualizar el progreso de cada usuario tanto en sus temáticas como en su álbum digital dentro de la informacion de cada perfil</t>
+  </si>
+  <si>
+    <t>Realizar la asignación aleatoria de las preguntas para cada usuario.</t>
+  </si>
+  <si>
+    <t>EPIC02-HU01
+EPIC02-HU02</t>
+  </si>
+  <si>
+    <t>Entregar los cromos al usuario, en concordancia con sus temáticas y en funcion de los aciertos del mismo.</t>
+  </si>
+  <si>
+    <t>Relacionar el perfil del usuario conjuntamente con su album digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validar la página principal del sistema web </t>
+  </si>
+  <si>
+    <t>Conocer su estructura y sus componentes</t>
+  </si>
+  <si>
+    <t>Visualizar el diseño preliminar de la página web principal</t>
+  </si>
+  <si>
+    <t>Aceptar y/o sugerir modificaciones de la misma</t>
+  </si>
+  <si>
+    <t>1. Presentar el wireframe, mockup
+2. Presentar la página web principal desplegada en un servidor local</t>
+  </si>
+  <si>
+    <t>Visualizar el diseño preliminar del album digital y los perfiles de usuario</t>
+  </si>
+  <si>
+    <t>1. Presentar el wireframe, mockup
+2. Presentar el diseño preliminar del album y los perfiles de usuario</t>
+  </si>
+  <si>
+    <t>En progreso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -485,29 +512,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="15">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -562,38 +568,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFCE4D6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -653,11 +629,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -746,9 +735,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -773,27 +759,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -827,77 +792,164 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="lightUp">
@@ -1514,34 +1566,34 @@
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:S80"/>
+  <dimension ref="B1:S77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="48" style="5" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="5" customWidth="1"/>
     <col min="7" max="7" width="19" style="4" customWidth="1"/>
-    <col min="8" max="8" width="56.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="23.5" style="4" customWidth="1"/>
-    <col min="10" max="10" width="53.1640625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="56.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="53.140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="5" customWidth="1"/>
     <col min="12" max="13" width="15" style="5" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="5" customWidth="1"/>
-    <col min="15" max="15" width="12.5" style="5" customWidth="1"/>
-    <col min="16" max="16" width="39.5" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="39.42578125" style="4" customWidth="1"/>
     <col min="17" max="17" width="6" style="6" customWidth="1"/>
-    <col min="18" max="16384" width="9.1640625" style="6"/>
+    <col min="18" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="18" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
@@ -1553,24 +1605,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="59" t="s">
+    <row r="2" spans="2:19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="52"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
       <c r="O2" s="29"/>
       <c r="P2" s="24"/>
       <c r="Q2" s="24"/>
@@ -1579,24 +1631,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="59" t="s">
+    <row r="3" spans="2:19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="60"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="52"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
       <c r="O3" s="29"/>
       <c r="P3" s="24"/>
       <c r="Q3" s="24"/>
@@ -1605,7 +1657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:19" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:19" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -1627,30 +1679,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B5" s="50" t="s">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B5" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="53" t="s">
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="56" t="s">
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="57"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="58"/>
-    </row>
-    <row r="6" spans="2:19" ht="28" x14ac:dyDescent="0.15">
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="50"/>
+    </row>
+    <row r="6" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="33" t="s">
         <v>10</v>
       </c>
@@ -1663,58 +1715,58 @@
       <c r="E6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="37" t="s">
+      <c r="I6" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="39" t="s">
+      <c r="K6" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="39" t="s">
+      <c r="L6" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="39" t="s">
+      <c r="M6" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="39" t="s">
+      <c r="N6" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="39" t="s">
+      <c r="O6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="38" t="s">
+      <c r="P6" s="37" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="42" x14ac:dyDescent="0.15">
-      <c r="B7" s="41" t="s">
+    <row r="7" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B7" s="40" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="42"/>
+        <v>76</v>
+      </c>
+      <c r="F7" s="41"/>
       <c r="G7" s="41"/>
-      <c r="H7" s="43"/>
+      <c r="H7" s="41"/>
       <c r="I7" s="41"/>
-      <c r="J7" s="34"/>
+      <c r="J7" s="9"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -1722,416 +1774,448 @@
       <c r="O7" s="8"/>
       <c r="P7" s="9"/>
     </row>
-    <row r="8" spans="2:19" ht="42" x14ac:dyDescent="0.15">
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71" t="s">
+    <row r="8" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" s="54">
+        <v>2</v>
+      </c>
+      <c r="L8" s="54">
+        <v>15</v>
+      </c>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54">
+        <v>1</v>
+      </c>
+      <c r="O8" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="P8" s="9"/>
+    </row>
+    <row r="9" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K9" s="54">
+        <v>2</v>
+      </c>
+      <c r="L9" s="54">
+        <v>15</v>
+      </c>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54">
+        <v>1</v>
+      </c>
+      <c r="O9" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="P9" s="9"/>
+    </row>
+    <row r="10" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="54"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+    </row>
+    <row r="11" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B11" s="41"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="71" t="s">
+      <c r="J11" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="54">
+        <v>1</v>
+      </c>
+      <c r="L11" s="54">
+        <v>25</v>
+      </c>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54">
+        <v>2</v>
+      </c>
+      <c r="O11" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" s="54"/>
+    </row>
+    <row r="12" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B12" s="41"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="71" t="s">
+      <c r="H12" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="54">
+        <v>1</v>
+      </c>
+      <c r="L12" s="54">
+        <v>25</v>
+      </c>
+      <c r="M12" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="N12" s="54">
+        <v>5</v>
+      </c>
+      <c r="O12" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="P12" s="54"/>
+    </row>
+    <row r="13" spans="2:19" ht="51" x14ac:dyDescent="0.2">
+      <c r="B13" s="8"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="54">
+        <v>1</v>
+      </c>
+      <c r="L13" s="54">
+        <v>20</v>
+      </c>
+      <c r="M13" s="54"/>
+      <c r="N13" s="54">
+        <v>5</v>
+      </c>
+      <c r="O13" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" s="54"/>
+    </row>
+    <row r="14" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B14" s="41"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="54">
+        <v>2</v>
+      </c>
+      <c r="L14" s="54">
+        <v>15</v>
+      </c>
+      <c r="M14" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="N14" s="54">
+        <v>2</v>
+      </c>
+      <c r="O14" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="54"/>
+    </row>
+    <row r="15" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B15" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="54"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
+    </row>
+    <row r="16" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B16" s="41"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" s="54">
+        <v>1</v>
+      </c>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54">
+        <v>4</v>
+      </c>
+      <c r="O16" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="P16" s="54"/>
+    </row>
+    <row r="17" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B17" s="41"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="72" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="73">
+      <c r="G17" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17" s="54">
         <v>1</v>
       </c>
-      <c r="L8" s="73">
-        <v>25</v>
-      </c>
-      <c r="M8" s="73"/>
-      <c r="N8" s="73">
+      <c r="L17" s="54"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54">
+        <v>3</v>
+      </c>
+      <c r="O17" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="P17" s="54"/>
+    </row>
+    <row r="18" spans="2:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B18" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="54"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+    </row>
+    <row r="19" spans="2:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B19" s="41"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="K19" s="54">
         <v>1</v>
       </c>
-      <c r="O8" s="73" t="s">
-        <v>5</v>
-      </c>
-      <c r="P8" s="61"/>
-    </row>
-    <row r="9" spans="2:19" ht="42" x14ac:dyDescent="0.15">
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" s="8">
+      <c r="L19" s="54"/>
+      <c r="M19" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="N19" s="54">
+        <v>2</v>
+      </c>
+      <c r="O19" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="8">
-        <v>25</v>
-      </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8">
-        <v>1</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="P9" s="9"/>
-    </row>
-    <row r="10" spans="2:19" ht="56" x14ac:dyDescent="0.15">
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="48">
-        <v>1</v>
-      </c>
-      <c r="L10" s="48">
-        <v>20</v>
-      </c>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48">
-        <v>2</v>
-      </c>
-      <c r="O10" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="P10" s="49"/>
-    </row>
-    <row r="11" spans="2:19" ht="42" x14ac:dyDescent="0.15">
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="K11" s="65">
-        <v>2</v>
-      </c>
-      <c r="L11" s="65">
-        <v>15</v>
-      </c>
-      <c r="M11" s="65" t="s">
-        <v>37</v>
-      </c>
-      <c r="N11" s="65">
-        <v>2</v>
-      </c>
-      <c r="O11" s="65" t="s">
-        <v>6</v>
-      </c>
-      <c r="P11" s="66"/>
-    </row>
-    <row r="12" spans="2:19" ht="42" x14ac:dyDescent="0.15">
-      <c r="B12" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="9"/>
-    </row>
-    <row r="13" spans="2:19" ht="42" x14ac:dyDescent="0.15">
-      <c r="B13" s="75"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="77" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="77" t="s">
-        <v>61</v>
-      </c>
-      <c r="J13" s="79" t="s">
-        <v>63</v>
-      </c>
-      <c r="K13" s="75">
-        <v>1</v>
-      </c>
-      <c r="L13" s="75"/>
-      <c r="M13" s="75"/>
-      <c r="N13" s="75">
-        <v>4</v>
-      </c>
-      <c r="O13" s="81" t="s">
-        <v>74</v>
-      </c>
-      <c r="P13" s="78"/>
-    </row>
-    <row r="14" spans="2:19" ht="28" x14ac:dyDescent="0.15">
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="68" t="s">
-        <v>60</v>
-      </c>
-      <c r="I14" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="K14" s="70">
-        <v>1</v>
-      </c>
-      <c r="L14" s="70"/>
-      <c r="M14" s="70"/>
-      <c r="N14" s="70">
-        <v>4</v>
-      </c>
-      <c r="O14" s="82" t="s">
-        <v>74</v>
-      </c>
-      <c r="P14" s="66"/>
-    </row>
-    <row r="15" spans="2:19" ht="28" x14ac:dyDescent="0.15">
-      <c r="B15" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="44"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="9"/>
-    </row>
-    <row r="16" spans="2:19" ht="28" x14ac:dyDescent="0.15">
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" s="77" t="s">
-        <v>69</v>
-      </c>
-      <c r="I16" s="77" t="s">
-        <v>71</v>
-      </c>
-      <c r="J16" s="79" t="s">
-        <v>73</v>
-      </c>
-      <c r="K16" s="75">
-        <v>1</v>
-      </c>
-      <c r="L16" s="75"/>
-      <c r="M16" s="75"/>
-      <c r="N16" s="75">
-        <v>5</v>
-      </c>
-      <c r="O16" s="81" t="s">
-        <v>74</v>
-      </c>
-      <c r="P16" s="78"/>
-    </row>
-    <row r="17" spans="2:16" ht="28" x14ac:dyDescent="0.15">
-      <c r="B17" s="67"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="H17" s="80" t="s">
-        <v>70</v>
-      </c>
-      <c r="I17" s="68" t="s">
-        <v>71</v>
-      </c>
-      <c r="J17" s="69" t="s">
-        <v>72</v>
-      </c>
-      <c r="K17" s="70">
-        <v>1</v>
-      </c>
-      <c r="L17" s="70"/>
-      <c r="M17" s="70"/>
-      <c r="N17" s="70">
-        <v>5</v>
-      </c>
-      <c r="O17" s="82" t="s">
-        <v>74</v>
-      </c>
-      <c r="P17" s="66"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="9"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="9"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="9"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="9"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="P19" s="54"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="54"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="9"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="F22" s="54"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
+      <c r="P22" s="54"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2148,15 +2232,15 @@
       <c r="O23" s="8"/>
       <c r="P23" s="9"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
@@ -2165,15 +2249,15 @@
       <c r="O24" s="8"/>
       <c r="P24" s="9"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
@@ -2182,472 +2266,393 @@
       <c r="O25" s="8"/>
       <c r="P25" s="9"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="9"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="9"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="9"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="9"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="9"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="9"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="9"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B33" s="42"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="9"/>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="9"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="9"/>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="9"/>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="9"/>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B38" s="42"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="9"/>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B39" s="42"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="42"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="9"/>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="42"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="9"/>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="9"/>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="9"/>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B43" s="42"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="9"/>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="9"/>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B45" s="42"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="9"/>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="9"/>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B47" s="42"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="9"/>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B48" s="42"/>
-      <c r="C48" s="42"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="9"/>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B49" s="42"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="9"/>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B50" s="42"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="42"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="9"/>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B51" s="42"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="42"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="8"/>
-      <c r="O51" s="8"/>
-      <c r="P51" s="9"/>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
-    </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="P69" s="7"/>
-    </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
-      <c r="H80" s="6"/>
-      <c r="I80" s="6"/>
-      <c r="J80" s="6"/>
-      <c r="K80" s="6"/>
-      <c r="L80" s="6"/>
-      <c r="M80" s="6"/>
-      <c r="N80" s="6"/>
-      <c r="O80" s="6"/>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B33" s="8"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B34" s="8"/>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B35" s="55"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="55"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="55"/>
+      <c r="N35" s="55"/>
+      <c r="O35" s="55"/>
+      <c r="P35" s="56"/>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="58"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="58"/>
+      <c r="Q36" s="59"/>
+      <c r="R36" s="59"/>
+      <c r="S36" s="59"/>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="58"/>
+      <c r="Q37" s="59"/>
+      <c r="R37" s="59"/>
+      <c r="S37" s="59"/>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="58"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="58"/>
+      <c r="Q38" s="59"/>
+      <c r="R38" s="59"/>
+      <c r="S38" s="59"/>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="57"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="57"/>
+      <c r="J39" s="58"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
+      <c r="O39" s="29"/>
+      <c r="P39" s="58"/>
+      <c r="Q39" s="59"/>
+      <c r="R39" s="59"/>
+      <c r="S39" s="59"/>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B40" s="57"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="57"/>
+      <c r="H40" s="57"/>
+      <c r="I40" s="57"/>
+      <c r="J40" s="58"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="58"/>
+      <c r="Q40" s="59"/>
+      <c r="R40" s="59"/>
+      <c r="S40" s="59"/>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B41" s="57"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="58"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="58"/>
+      <c r="Q41" s="59"/>
+      <c r="R41" s="59"/>
+      <c r="S41" s="59"/>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="58"/>
+      <c r="Q42" s="59"/>
+      <c r="R42" s="59"/>
+      <c r="S42" s="59"/>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="59"/>
+      <c r="R43" s="59"/>
+      <c r="S43" s="59"/>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B44" s="57"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="58"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="58"/>
+      <c r="Q44" s="59"/>
+      <c r="R44" s="59"/>
+      <c r="S44" s="59"/>
+    </row>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="58"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="29"/>
+      <c r="M45" s="29"/>
+      <c r="N45" s="29"/>
+      <c r="O45" s="29"/>
+      <c r="P45" s="58"/>
+      <c r="Q45" s="59"/>
+      <c r="R45" s="59"/>
+      <c r="S45" s="59"/>
+    </row>
+    <row r="46" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="29"/>
+      <c r="L46" s="29"/>
+      <c r="M46" s="29"/>
+      <c r="N46" s="29"/>
+      <c r="O46" s="29"/>
+      <c r="P46" s="58"/>
+      <c r="Q46" s="59"/>
+      <c r="R46" s="59"/>
+      <c r="S46" s="59"/>
+    </row>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B47" s="57"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="58"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="29"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
+      <c r="O47" s="29"/>
+      <c r="P47" s="58"/>
+      <c r="Q47" s="59"/>
+      <c r="R47" s="59"/>
+      <c r="S47" s="59"/>
+    </row>
+    <row r="48" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B48" s="57"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="57"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="29"/>
+      <c r="L48" s="29"/>
+      <c r="M48" s="29"/>
+      <c r="N48" s="29"/>
+      <c r="O48" s="29"/>
+      <c r="P48" s="58"/>
+      <c r="Q48" s="59"/>
+      <c r="R48" s="59"/>
+      <c r="S48" s="59"/>
+    </row>
+    <row r="49" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="58"/>
+      <c r="I49" s="58"/>
+      <c r="J49" s="58"/>
+      <c r="K49" s="29"/>
+      <c r="L49" s="29"/>
+      <c r="M49" s="29"/>
+      <c r="N49" s="29"/>
+      <c r="O49" s="29"/>
+      <c r="P49" s="58"/>
+      <c r="Q49" s="59"/>
+      <c r="R49" s="59"/>
+      <c r="S49" s="59"/>
+    </row>
+    <row r="50" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="58"/>
+      <c r="J50" s="58"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="58"/>
+      <c r="Q50" s="59"/>
+      <c r="R50" s="59"/>
+      <c r="S50" s="59"/>
+    </row>
+    <row r="51" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="58"/>
+      <c r="H51" s="58"/>
+      <c r="I51" s="58"/>
+      <c r="J51" s="58"/>
+      <c r="K51" s="29"/>
+      <c r="L51" s="29"/>
+      <c r="M51" s="29"/>
+      <c r="N51" s="29"/>
+      <c r="O51" s="29"/>
+      <c r="P51" s="58"/>
+      <c r="Q51" s="59"/>
+      <c r="R51" s="59"/>
+      <c r="S51" s="59"/>
+    </row>
+    <row r="52" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="58"/>
+      <c r="I52" s="58"/>
+      <c r="J52" s="58"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="29"/>
+      <c r="M52" s="29"/>
+      <c r="N52" s="29"/>
+      <c r="O52" s="29"/>
+      <c r="P52" s="58"/>
+      <c r="Q52" s="59"/>
+      <c r="R52" s="59"/>
+      <c r="S52" s="59"/>
+    </row>
+    <row r="53" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P66" s="7"/>
+    </row>
+    <row r="77" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="6"/>
+      <c r="N77" s="6"/>
+      <c r="O77" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2660,99 +2665,132 @@
     <mergeCell ref="D3:E3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="P69:P70">
-    <cfRule type="expression" dxfId="30" priority="25" stopIfTrue="1">
+  <conditionalFormatting sqref="P66:P67">
+    <cfRule type="expression" dxfId="48" priority="58" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="59" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="60" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P24">
-    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
-      <formula>#REF!="Done"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="29" stopIfTrue="1">
-      <formula>#REF!="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="30" stopIfTrue="1">
-      <formula>#REF!="Removed"</formula>
+  <conditionalFormatting sqref="P77">
+    <cfRule type="expression" dxfId="42" priority="106" stopIfTrue="1">
+      <formula>$O67="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="107" stopIfTrue="1">
+      <formula>$O67="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="108" stopIfTrue="1">
+      <formula>$O67="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P80">
-    <cfRule type="expression" dxfId="24" priority="73" stopIfTrue="1">
-      <formula>$O70="Done"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="74" stopIfTrue="1">
-      <formula>$O70="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="75" stopIfTrue="1">
-      <formula>$O70="Removed"</formula>
+  <conditionalFormatting sqref="B21:E21 B36:P122 C7:P7 C10:E12">
+    <cfRule type="expression" dxfId="39" priority="64" stopIfTrue="1">
+      <formula>$O7="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="65" stopIfTrue="1">
+      <formula>$O7="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="66" stopIfTrue="1">
+      <formula>$O7="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:G7 I7 B8:J12 C13:J13 K7:P20 B14:J14 B24:P125 C15:J15 B18:J20 B16:G17 I16:J17">
-    <cfRule type="expression" dxfId="21" priority="31" stopIfTrue="1">
-      <formula>$O7="Terminado"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="32" stopIfTrue="1">
-      <formula>$O7="En Progreso"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="33" stopIfTrue="1">
-      <formula>$O7="Eliminado"</formula>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="expression" dxfId="33" priority="172" stopIfTrue="1">
+      <formula>$O15="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="173" stopIfTrue="1">
+      <formula>$O15="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="174" stopIfTrue="1">
+      <formula>$O15="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3">
-    <cfRule type="expression" dxfId="18" priority="79" stopIfTrue="1">
-      <formula>$O11="Done"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="80" stopIfTrue="1">
-      <formula>$O11="In Progress"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="81" stopIfTrue="1">
-      <formula>$O11="Removed"</formula>
+  <conditionalFormatting sqref="R3 R1">
+    <cfRule type="expression" dxfId="20" priority="208" stopIfTrue="1">
+      <formula>$O12="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="209" stopIfTrue="1">
+      <formula>$O12="In Progress"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="210" stopIfTrue="1">
+      <formula>$O12="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R1">
-    <cfRule type="expression" dxfId="15" priority="82" stopIfTrue="1">
-      <formula>$O9="Done"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="83" stopIfTrue="1">
-      <formula>$O9="In Progress"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="84" stopIfTrue="1">
-      <formula>$O9="Removed"</formula>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="expression" dxfId="17" priority="214" stopIfTrue="1">
+      <formula>$O10="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="215" stopIfTrue="1">
+      <formula>$O10="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="216" stopIfTrue="1">
+      <formula>$O10="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="12" priority="88" stopIfTrue="1">
-      <formula>$O13="Terminado"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="89" stopIfTrue="1">
-      <formula>$O13="En Progreso"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="90" stopIfTrue="1">
-      <formula>$O13="Eliminado"</formula>
+  <conditionalFormatting sqref="B11:B12">
+    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
+      <formula>$O16="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+      <formula>$O16="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
+      <formula>$O16="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
-    <cfRule type="expression" dxfId="2" priority="94" stopIfTrue="1">
-      <formula>$O17="Terminado"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="95" stopIfTrue="1">
-      <formula>$O17="En Progreso"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="96" stopIfTrue="1">
-      <formula>$O17="Eliminado"</formula>
+  <conditionalFormatting sqref="C14:E14">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+      <formula>$O14="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+      <formula>$O14="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+      <formula>$O14="Eliminado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+      <formula>$O19="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+      <formula>$O19="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
+      <formula>$O19="Eliminado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:E19">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+      <formula>$O15="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+      <formula>$O15="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+      <formula>$O15="Eliminado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:B19">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+      <formula>$O20="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
+      <formula>$O20="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
+      <formula>$O20="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="O81:O190 O24:O79 O6:O20" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="O78:O187 O35:O76 O6:O19 O21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Por Hacer,En Progreso,Terminado,Eliminado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K24:K51 K7:K20" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K35:K48 K7:K19 K21" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2769,36 +2807,36 @@
   <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="22" style="2" customWidth="1"/>
-    <col min="9" max="9" width="59.1640625" customWidth="1"/>
+    <col min="9" max="9" width="59.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" s="26" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>20</v>
@@ -2807,137 +2845,129 @@
         <v>23</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="17">
         <v>1</v>
       </c>
-      <c r="C3" s="36">
-        <v>43332</v>
+      <c r="C3" s="35">
+        <v>44160</v>
       </c>
       <c r="D3" s="20">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E3" s="21">
-        <v>43362</v>
+        <v>44167</v>
       </c>
       <c r="F3" s="17">
-        <f>IF(B3="","",SUMIF('Backlog del Producto'!N$7:N$130,Sprints!B3,'Backlog del Producto'!L$7:L$130))</f>
-        <v>50</v>
+        <f>IF(B3="","",SUMIF('Backlog del Producto'!N$21:N$127,Sprints!B3,'Backlog del Producto'!L$21:L$127))</f>
+        <v>0</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="17">
         <v>2</v>
       </c>
       <c r="C4" s="19">
-        <f>IF(AND(C3&lt;&gt;"",D3&lt;&gt;"",D4&lt;&gt;""),C3+D3,"")</f>
-        <v>43362</v>
+        <v>44168</v>
       </c>
       <c r="D4" s="20">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E4" s="21">
-        <f>IF(AND(C4&lt;&gt;"",D4&lt;&gt;""),C4+D4-1,"")</f>
-        <v>43376</v>
+        <v>44178</v>
       </c>
       <c r="F4" s="17">
-        <f>IF(B4="","",SUMIF('Backlog del Producto'!N$7:N$130,Sprints!B4,'Backlog del Producto'!L$7:L$130))</f>
-        <v>35</v>
+        <f>IF(B4="","",SUMIF('Backlog del Producto'!N$21:N$127,Sprints!B4,'Backlog del Producto'!L$21:L$127))</f>
+        <v>0</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="17">
         <v>3</v>
       </c>
       <c r="C5" s="19">
-        <f>IF(AND(C4&lt;&gt;"",D4&lt;&gt;"",D5&lt;&gt;""),C4+D4,"")</f>
-        <v>43377</v>
+        <v>44179</v>
       </c>
       <c r="D5" s="20">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E5" s="21">
-        <f>IF(AND(C5&lt;&gt;"",D5&lt;&gt;""),C5+D5-1,"")</f>
-        <v>43406</v>
+        <v>44194</v>
       </c>
       <c r="F5" s="17">
-        <f>IF(B5="","",SUMIF('Backlog del Producto'!N$7:N$130,Sprints!B5,'Backlog del Producto'!L$7:L$130))</f>
+        <f>IF(B5="","",SUMIF('Backlog del Producto'!N$21:N$127,Sprints!B5,'Backlog del Producto'!L$21:L$127))</f>
         <v>0</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="15"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="17">
         <v>4</v>
       </c>
       <c r="C6" s="19">
-        <f>IF(AND(C5&lt;&gt;"",D5&lt;&gt;"",D6&lt;&gt;""),C5+D5,"")</f>
-        <v>43407</v>
+        <v>44200</v>
       </c>
       <c r="D6" s="20">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E6" s="21">
-        <f>IF(AND(C6&lt;&gt;"",D6&lt;&gt;""),C6+D6-1,"")</f>
-        <v>43436</v>
+        <v>44215</v>
       </c>
       <c r="F6" s="17">
-        <f>IF(B6="","",SUMIF('Backlog del Producto'!N$7:N$130,Sprints!B6,'Backlog del Producto'!L$7:L$130))</f>
+        <f>IF(B6="","",SUMIF('Backlog del Producto'!N$21:N$127,Sprints!B6,'Backlog del Producto'!L$21:L$127))</f>
         <v>0</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="15"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="17">
         <v>5</v>
       </c>
       <c r="C7" s="19">
-        <f>IF(AND(C6&lt;&gt;"",D6&lt;&gt;"",D7&lt;&gt;""),C6+D6,"")</f>
-        <v>43437</v>
+        <v>44230</v>
       </c>
       <c r="D7" s="20">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E7" s="21">
-        <f>IF(AND(C7&lt;&gt;"",D7&lt;&gt;""),C7+D7-1,"")</f>
-        <v>43466</v>
+        <v>44245</v>
       </c>
       <c r="F7" s="17">
-        <f>IF(B7="","",SUMIF('Backlog del Producto'!N$7:N$130,Sprints!B7,'Backlog del Producto'!L$7:L$130))</f>
+        <f>IF(B7="","",SUMIF('Backlog del Producto'!N$21:N$127,Sprints!B7,'Backlog del Producto'!L$21:L$127))</f>
         <v>0</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="17"/>
       <c r="C8" s="19"/>
       <c r="D8" s="20"/>
@@ -2947,7 +2977,7 @@
       <c r="H8" s="20"/>
       <c r="I8" s="15"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="str">
         <f t="shared" ref="B9:B17" si="0">IF(AND(C9&lt;&gt;"",D9&lt;&gt;""),B8+1,"")</f>
         <v/>
@@ -2962,7 +2992,7 @@
         <v/>
       </c>
       <c r="F9" s="17" t="str">
-        <f>IF(B9="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B9,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B9="","",SUMIF('Backlog del Producto'!N$11:N$127,Sprints!B9,'Backlog del Producto'!L$11:L$127))</f>
         <v/>
       </c>
       <c r="G9" s="18" t="str">
@@ -2972,7 +3002,7 @@
       <c r="H9" s="20"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2987,7 +3017,7 @@
         <v/>
       </c>
       <c r="F10" s="17" t="str">
-        <f>IF(B10="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B10,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B10="","",SUMIF('Backlog del Producto'!N$11:N$127,Sprints!B10,'Backlog del Producto'!L$11:L$127))</f>
         <v/>
       </c>
       <c r="G10" s="18" t="str">
@@ -2997,7 +3027,7 @@
       <c r="H10" s="20"/>
       <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3012,7 +3042,7 @@
         <v/>
       </c>
       <c r="F11" s="17" t="str">
-        <f>IF(B11="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B11,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B11="","",SUMIF('Backlog del Producto'!N$11:N$127,Sprints!B11,'Backlog del Producto'!L$11:L$127))</f>
         <v/>
       </c>
       <c r="G11" s="18" t="str">
@@ -3022,7 +3052,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="15"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3037,7 +3067,7 @@
         <v/>
       </c>
       <c r="F12" s="17" t="str">
-        <f>IF(B12="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B12,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B12="","",SUMIF('Backlog del Producto'!N$11:N$127,Sprints!B12,'Backlog del Producto'!L$11:L$127))</f>
         <v/>
       </c>
       <c r="G12" s="18" t="str">
@@ -3047,7 +3077,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="15"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3062,7 +3092,7 @@
         <v/>
       </c>
       <c r="F13" s="17" t="str">
-        <f>IF(B13="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B13,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B13="","",SUMIF('Backlog del Producto'!N$11:N$127,Sprints!B13,'Backlog del Producto'!L$11:L$127))</f>
         <v/>
       </c>
       <c r="G13" s="18" t="str">
@@ -3072,7 +3102,7 @@
       <c r="H13" s="20"/>
       <c r="I13" s="15"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3087,7 +3117,7 @@
         <v/>
       </c>
       <c r="F14" s="17" t="str">
-        <f>IF(B14="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B14,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B14="","",SUMIF('Backlog del Producto'!N$11:N$127,Sprints!B14,'Backlog del Producto'!L$11:L$127))</f>
         <v/>
       </c>
       <c r="G14" s="18" t="str">
@@ -3097,7 +3127,7 @@
       <c r="H14" s="20"/>
       <c r="I14" s="15"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3112,7 +3142,7 @@
         <v/>
       </c>
       <c r="F15" s="17" t="str">
-        <f>IF(B15="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B15,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B15="","",SUMIF('Backlog del Producto'!N$11:N$127,Sprints!B15,'Backlog del Producto'!L$11:L$127))</f>
         <v/>
       </c>
       <c r="G15" s="18" t="str">
@@ -3122,7 +3152,7 @@
       <c r="H15" s="20"/>
       <c r="I15" s="15"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3137,7 +3167,7 @@
         <v/>
       </c>
       <c r="F16" s="17" t="str">
-        <f>IF(B16="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B16,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B16="","",SUMIF('Backlog del Producto'!N$11:N$127,Sprints!B16,'Backlog del Producto'!L$11:L$127))</f>
         <v/>
       </c>
       <c r="G16" s="18" t="str">
@@ -3147,7 +3177,7 @@
       <c r="H16" s="20"/>
       <c r="I16" s="15"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3162,7 +3192,7 @@
         <v/>
       </c>
       <c r="F17" s="17" t="str">
-        <f>IF(B17="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B17,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B17="","",SUMIF('Backlog del Producto'!N$11:N$127,Sprints!B17,'Backlog del Producto'!L$11:L$127))</f>
         <v/>
       </c>
       <c r="G17" s="18" t="str">
@@ -3172,16 +3202,16 @@
       <c r="H17" s="20"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="14"/>
       <c r="E18" s="22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F18" s="17">
-        <f>SUMIF('Backlog del Producto'!N$8:N$130,"",'Backlog del Producto'!L$8:L$130)-SUMIF('Backlog del Producto'!O$8:O$130,"Eliminado",'Backlog del Producto'!L$8:L$130)</f>
-        <v>-15</v>
+        <f>SUMIF('Backlog del Producto'!N$11:N$127,"",'Backlog del Producto'!L$11:L$127)-SUMIF('Backlog del Producto'!O$11:O$127,"Eliminado",'Backlog del Producto'!L$11:L$127)</f>
+        <v>0</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="23"/>
@@ -3190,29 +3220,29 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="9" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="1" stopIfTrue="1">
       <formula>$G18="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="2" stopIfTrue="1">
       <formula>$G18="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G17">
-    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="3" stopIfTrue="1">
       <formula>$G3="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="4" stopIfTrue="1">
       <formula>$G3="Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Unplanned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:I17 B3:F17">
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
       <formula>OR($G3="Planned",$G3="Unplanned")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="7" stopIfTrue="1">
       <formula>$G3="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3228,6 +3258,60 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A5124E24CAF14D46B2DD609ACFD84C07" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9971b3b784abbe199b171e233c6d3889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="01eb4bd6-a8ff-4439-b7eb-fe0a650fbd8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a36e787f936117f0a8f63b0cc0186e7" ns2:_="">
     <xsd:import namespace="01eb4bd6-a8ff-4439-b7eb-fe0a650fbd8a"/>
@@ -3372,67 +3456,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3441,7 +3465,29 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09A1246-53BD-4D90-8F0D-F04270C7DF7F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617ABD26-2811-4761-B5CB-14D5621085A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3459,35 +3505,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09A1246-53BD-4D90-8F0D-F04270C7DF7F}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A0D1E8-B670-4184-80F1-6022252F7605}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Arreglo N2 27 noviembre, backlog
</commit_message>
<xml_diff>
--- a/documetacionSoftware/1. Inicio/Backlog del producto.xlsx
+++ b/documetacionSoftware/1. Inicio/Backlog del producto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sant Garcia\Documents\5to Ciclo\proyectoCromos\documetacionSoftware\1. Inicio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53373C5-FF01-43EA-AD1A-88B004683ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93096193-9D76-454C-932C-797F0BE3C16A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="88">
   <si>
     <t>Backlog del Producto</t>
   </si>
@@ -397,9 +397,6 @@
 3. Confirmar la existencia del correo mediante una URL enviada al mismo</t>
   </si>
   <si>
-    <t>Gestor de usuarios</t>
-  </si>
-  <si>
     <t>Modificar los datos de un usuario ya existente en el sistema, tales como nombre y apellido, nickname, pais, edad, contraseña</t>
   </si>
   <si>
@@ -418,18 +415,12 @@
 4. Registro de nueva contraseña en la base de datos del sistema</t>
   </si>
   <si>
-    <t>Gestor de banco de preguntas</t>
-  </si>
-  <si>
     <t>HU05</t>
   </si>
   <si>
     <t>Controlar la distribución de las preguntas, para cada usuario</t>
   </si>
   <si>
-    <t>Gestor de cromos</t>
-  </si>
-  <si>
     <t>Controlar la distribución de los cromos para los usuarios</t>
   </si>
   <si>
@@ -446,9 +437,6 @@
   </si>
   <si>
     <t>Mantener una estructura similar y organizada</t>
-  </si>
-  <si>
-    <t>Gestor de álbum</t>
   </si>
   <si>
     <t>Clasificar las páginas del álbum mediante las seis temáticas existentes</t>
@@ -472,6 +460,15 @@
   <si>
     <t>1. Asignar cada pregunta a una tematica
 2. Guardar cada pregunta dentro del sistema</t>
+  </si>
+  <si>
+    <t>Dueño del producto</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Administradores</t>
   </si>
 </sst>
 </file>
@@ -836,7 +833,161 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="64">
+  <dxfs count="73">
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -888,94 +1039,6 @@
         <extend val="0"/>
         <color indexed="54"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1697,8 +1760,8 @@
   </sheetPr>
   <dimension ref="B1:S73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1883,7 +1946,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>56</v>
@@ -1911,8 +1974,8 @@
       <c r="F8" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="41" t="s">
-        <v>66</v>
+      <c r="G8" s="40" t="s">
+        <v>85</v>
       </c>
       <c r="H8" s="41" t="s">
         <v>61</v>
@@ -1946,17 +2009,17 @@
       <c r="F9" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="41" t="s">
         <v>66</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>67</v>
       </c>
       <c r="I9" s="41" t="s">
         <v>64</v>
       </c>
       <c r="J9" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K9" s="43">
         <v>1</v>
@@ -1981,17 +2044,17 @@
       <c r="F10" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="41" t="s">
-        <v>66</v>
+      <c r="G10" s="40" t="s">
+        <v>86</v>
       </c>
       <c r="H10" s="41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" s="41" t="s">
         <v>64</v>
       </c>
       <c r="J10" s="41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K10" s="43">
         <v>1</v>
@@ -2017,7 +2080,7 @@
         <v>36</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="H11" s="41" t="s">
         <v>63</v>
@@ -2049,10 +2112,10 @@
       <c r="D12" s="42"/>
       <c r="E12" s="42"/>
       <c r="F12" s="47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="H12" s="41" t="s">
         <v>58</v>
@@ -2085,10 +2148,10 @@
         <v>39</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E13" s="40"/>
       <c r="F13" s="47"/>
@@ -2112,16 +2175,16 @@
         <v>28</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="H14" s="49" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I14" s="40" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J14" s="40" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K14" s="43">
         <v>1</v>
@@ -2145,10 +2208,10 @@
         <v>30</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I15" s="41" t="s">
         <v>31</v>
@@ -2178,7 +2241,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="D16" s="40" t="s">
         <v>57</v>
@@ -2207,10 +2270,10 @@
         <v>28</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H17" s="40" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I17" s="41" t="s">
         <v>53</v>
@@ -2242,16 +2305,16 @@
         <v>30</v>
       </c>
       <c r="G18" s="40" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H18" s="40" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I18" s="40" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J18" s="40" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="K18" s="43">
         <v>2</v>
@@ -2272,10 +2335,10 @@
         <v>26</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9"/>
@@ -2298,16 +2361,16 @@
         <v>28</v>
       </c>
       <c r="G20" s="40" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="H20" s="40" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I20" s="40" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J20" s="40" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K20" s="43">
         <v>2</v>
@@ -2332,11 +2395,11 @@
       <c r="F21" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="41" t="s">
-        <v>74</v>
+      <c r="G21" s="40" t="s">
+        <v>85</v>
       </c>
       <c r="H21" s="40" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I21" s="41" t="s">
         <v>34</v>
@@ -2826,175 +2889,252 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="P62:P63">
-    <cfRule type="expression" dxfId="63" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="89" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="90" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P73">
-    <cfRule type="expression" dxfId="60" priority="115" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="136" stopIfTrue="1">
       <formula>$O63="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="137" stopIfTrue="1">
       <formula>$O63="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="117" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="138" stopIfTrue="1">
       <formula>$O63="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:P118 C15:E17 C7:E11 B7">
-    <cfRule type="expression" dxfId="57" priority="73" stopIfTrue="1">
+  <conditionalFormatting sqref="B32:P118 C15:E15 C7:E11 B7 C17:E17 D16:E16">
+    <cfRule type="expression" dxfId="66" priority="94" stopIfTrue="1">
       <formula>$O7="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="95" stopIfTrue="1">
       <formula>$O7="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="96" stopIfTrue="1">
       <formula>$O7="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1">
-    <cfRule type="expression" dxfId="54" priority="217" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="238" stopIfTrue="1">
       <formula>$O15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="218" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="239" stopIfTrue="1">
       <formula>$O15="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="219" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="240" stopIfTrue="1">
       <formula>$O15="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12:E14">
-    <cfRule type="expression" dxfId="48" priority="235" stopIfTrue="1">
+  <conditionalFormatting sqref="C12:E12 C14:E14 D13:E13">
+    <cfRule type="expression" dxfId="60" priority="256" stopIfTrue="1">
       <formula>#REF!="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="236" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="257" stopIfTrue="1">
       <formula>#REF!="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="237" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="258" stopIfTrue="1">
       <formula>#REF!="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="42" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="28" stopIfTrue="1">
       <formula>$O22="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="29" stopIfTrue="1">
       <formula>$O22="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="30" stopIfTrue="1">
       <formula>$O22="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="expression" dxfId="39" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="25" stopIfTrue="1">
       <formula>$O27="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="26" stopIfTrue="1">
       <formula>$O27="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="27" stopIfTrue="1">
       <formula>$O27="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:E19">
-    <cfRule type="expression" dxfId="36" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="22" stopIfTrue="1">
       <formula>$O19="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="23" stopIfTrue="1">
       <formula>$O19="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="24" stopIfTrue="1">
       <formula>$O19="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17 B15">
-    <cfRule type="expression" dxfId="33" priority="256" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="277" stopIfTrue="1">
       <formula>#REF!="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="257" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="278" stopIfTrue="1">
       <formula>#REF!="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="258" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="279" stopIfTrue="1">
       <formula>#REF!="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="27" priority="265" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="286" stopIfTrue="1">
       <formula>#REF!="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="266" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="287" stopIfTrue="1">
       <formula>#REF!="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="267" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="288" stopIfTrue="1">
       <formula>#REF!="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B14">
-    <cfRule type="expression" dxfId="24" priority="283" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="304" stopIfTrue="1">
       <formula>$O16="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="284" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="305" stopIfTrue="1">
       <formula>$O16="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="285" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="306" stopIfTrue="1">
       <formula>$O16="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="18" priority="298" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="319" stopIfTrue="1">
       <formula>$O14="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="299" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="320" stopIfTrue="1">
       <formula>$O14="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="300" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="321" stopIfTrue="1">
       <formula>$O14="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="15" priority="307" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="328" stopIfTrue="1">
       <formula>#REF!="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="308" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="329" stopIfTrue="1">
       <formula>#REF!="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="309" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="330" stopIfTrue="1">
       <formula>#REF!="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="12" priority="310" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="331" stopIfTrue="1">
       <formula>#REF!="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="311" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="332" stopIfTrue="1">
       <formula>#REF!="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="312" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="333" stopIfTrue="1">
       <formula>#REF!="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3">
-    <cfRule type="expression" dxfId="9" priority="328" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="349" stopIfTrue="1">
       <formula>$O12="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="329" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="350" stopIfTrue="1">
       <formula>$O12="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="330" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="351" stopIfTrue="1">
       <formula>$O12="Removed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="expression" dxfId="20" priority="19" stopIfTrue="1">
+      <formula>$O8="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+      <formula>$O8="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
+      <formula>$O8="Eliminado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="expression" dxfId="17" priority="16" stopIfTrue="1">
+      <formula>$O9="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
+      <formula>$O9="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
+      <formula>$O9="Eliminado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
+      <formula>$O10="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+      <formula>$O10="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
+      <formula>$O10="Eliminado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
+      <formula>$O13="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+      <formula>$O13="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+      <formula>$O13="Eliminado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
+      <formula>$O16="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+      <formula>$O16="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
+      <formula>$O16="Eliminado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+      <formula>$O18="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+      <formula>$O18="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+      <formula>$O18="Eliminado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>$O21="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>$O21="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+      <formula>$O21="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="O74:O183 O31:O72 O21 O6:O12 O13:O17" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="O74:O183 O31:O72 O21 O6:O17" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Por Hacer,En Progreso,Terminado,Eliminado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K31:K44 K21 K7:K12 K13:K17" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K31:K44 K21 K7:K17" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3424,29 +3564,29 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="1" stopIfTrue="1">
       <formula>$G18="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="2" stopIfTrue="1">
       <formula>$G18="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G17">
-    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="3" stopIfTrue="1">
       <formula>$G3="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="4" stopIfTrue="1">
       <formula>$G3="Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Unplanned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:I17 B3:F17">
-    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
       <formula>OR($G3="Planned",$G3="Unplanned")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="7" stopIfTrue="1">
       <formula>$G3="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3462,60 +3602,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A5124E24CAF14D46B2DD609ACFD84C07" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9971b3b784abbe199b171e233c6d3889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="01eb4bd6-a8ff-4439-b7eb-fe0a650fbd8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a36e787f936117f0a8f63b0cc0186e7" ns2:_="">
     <xsd:import namespace="01eb4bd6-a8ff-4439-b7eb-fe0a650fbd8a"/>
@@ -3660,7 +3746,67 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3669,29 +3815,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09A1246-53BD-4D90-8F0D-F04270C7DF7F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617ABD26-2811-4761-B5CB-14D5621085A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3709,19 +3833,35 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09A1246-53BD-4D90-8F0D-F04270C7DF7F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A0D1E8-B670-4184-80F1-6022252F7605}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>